<commit_message>
Mise à jour de paramètres
Changement dans supplément CPP, MAx CPP  and QPP benefits, COLA. Ajout de documents dans dossier "docs".
</commit_message>
<xml_diff>
--- a/params/qpp_history.xlsx
+++ b/params/qpp_history.xlsx
@@ -1,21 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaud/cpp/params/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeielonelmezil/cpp/params/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4796F935-819A-184D-83EA-9327AB25BB04}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE49BAC9-6000-8546-8770-A1C5BB158F4F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5380" yWindow="1160" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="680" yWindow="460" windowWidth="18720" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="qppyear" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017" calcOnSave="0"/>
+  <calcPr calcId="179021" calcOnSave="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -113,6 +120,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -596,7 +607,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -605,6 +616,9 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -963,10 +977,10 @@
   <dimension ref="A1:AC68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1075,20 +1089,20 @@
       <c r="C2" s="6">
         <v>600</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="10">
         <f>D2+E2</f>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G2" s="6">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6">
+      <c r="G2" s="10">
+        <v>0</v>
+      </c>
+      <c r="H2" s="10">
         <v>0</v>
       </c>
       <c r="I2" s="6">
@@ -1112,10 +1126,10 @@
       <c r="O2" s="6">
         <v>0</v>
       </c>
-      <c r="P2" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="7">
+      <c r="P2" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="5">
         <v>0</v>
       </c>
       <c r="R2" s="6">
@@ -1124,10 +1138,10 @@
       <c r="S2" s="6">
         <v>65</v>
       </c>
-      <c r="T2" s="6">
+      <c r="T2" s="10">
         <v>0.375</v>
       </c>
-      <c r="U2" s="6">
+      <c r="U2" s="10">
         <v>0.6</v>
       </c>
       <c r="V2" s="6">
@@ -1139,10 +1153,10 @@
       <c r="X2" s="6">
         <v>70</v>
       </c>
-      <c r="Y2" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="6">
+      <c r="Y2" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="9">
         <v>0</v>
       </c>
       <c r="AA2" s="6">
@@ -1165,20 +1179,20 @@
       <c r="C3" s="6">
         <v>600</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="10">
         <f t="shared" ref="F3:F54" si="0">D3+E3</f>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G3" s="6">
-        <v>0</v>
-      </c>
-      <c r="H3" s="6">
+      <c r="G3" s="10">
+        <v>0</v>
+      </c>
+      <c r="H3" s="10">
         <v>0</v>
       </c>
       <c r="I3" s="6">
@@ -1202,11 +1216,11 @@
       <c r="O3" s="6">
         <v>0</v>
       </c>
-      <c r="P3" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="7">
-        <v>0</v>
+      <c r="P3" s="1">
+        <v>239.64</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>239.64</v>
       </c>
       <c r="R3" s="6">
         <v>45</v>
@@ -1214,10 +1228,10 @@
       <c r="S3" s="6">
         <v>65</v>
       </c>
-      <c r="T3" s="6">
+      <c r="T3" s="10">
         <v>0.375</v>
       </c>
-      <c r="U3" s="6">
+      <c r="U3" s="10">
         <v>0.6</v>
       </c>
       <c r="V3" s="6">
@@ -1229,10 +1243,10 @@
       <c r="X3" s="6">
         <v>70</v>
       </c>
-      <c r="Y3" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="6">
+      <c r="Y3" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="9">
         <v>0</v>
       </c>
       <c r="AA3" s="6">
@@ -1255,20 +1269,20 @@
       <c r="C4" s="6">
         <v>600</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="10">
         <f t="shared" si="0"/>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G4" s="6">
-        <v>0</v>
-      </c>
-      <c r="H4" s="6">
+      <c r="G4" s="10">
+        <v>0</v>
+      </c>
+      <c r="H4" s="10">
         <v>0</v>
       </c>
       <c r="I4" s="6">
@@ -1292,11 +1306,11 @@
       <c r="O4" s="6">
         <v>25.5</v>
       </c>
-      <c r="P4" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="7">
-        <v>0</v>
+      <c r="P4" s="1">
+        <v>366.96</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>366.96</v>
       </c>
       <c r="R4" s="6">
         <v>45</v>
@@ -1304,10 +1318,10 @@
       <c r="S4" s="6">
         <v>65</v>
       </c>
-      <c r="T4" s="6">
+      <c r="T4" s="10">
         <v>0.375</v>
       </c>
-      <c r="U4" s="6">
+      <c r="U4" s="10">
         <v>0.6</v>
       </c>
       <c r="V4" s="6">
@@ -1319,10 +1333,10 @@
       <c r="X4" s="6">
         <v>70</v>
       </c>
-      <c r="Y4" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="6">
+      <c r="Y4" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="9">
         <v>0</v>
       </c>
       <c r="AA4" s="6">
@@ -1345,20 +1359,20 @@
       <c r="C5" s="6">
         <v>600</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="10">
         <f t="shared" si="0"/>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6">
+      <c r="G5" s="10">
+        <v>0</v>
+      </c>
+      <c r="H5" s="10">
         <v>0</v>
       </c>
       <c r="I5" s="6">
@@ -1382,11 +1396,11 @@
       <c r="O5" s="6">
         <v>26.01</v>
       </c>
-      <c r="P5" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="7">
-        <v>0</v>
+      <c r="P5" s="1">
+        <v>499.44</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>499.44</v>
       </c>
       <c r="R5" s="6">
         <v>45</v>
@@ -1394,10 +1408,10 @@
       <c r="S5" s="6">
         <v>65</v>
       </c>
-      <c r="T5" s="6">
+      <c r="T5" s="10">
         <v>0.375</v>
       </c>
-      <c r="U5" s="6">
+      <c r="U5" s="10">
         <v>0.6</v>
       </c>
       <c r="V5" s="6">
@@ -1409,10 +1423,10 @@
       <c r="X5" s="6">
         <v>70</v>
       </c>
-      <c r="Y5" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="6">
+      <c r="Y5" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="9">
         <v>0</v>
       </c>
       <c r="AA5" s="6">
@@ -1435,20 +1449,20 @@
       <c r="C6" s="6">
         <v>600</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="10">
         <f t="shared" si="0"/>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G6" s="6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="6">
+      <c r="G6" s="10">
+        <v>0</v>
+      </c>
+      <c r="H6" s="10">
         <v>0</v>
       </c>
       <c r="I6" s="6">
@@ -1472,11 +1486,11 @@
       <c r="O6" s="6">
         <v>26.53</v>
       </c>
-      <c r="P6" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="7">
-        <v>0</v>
+      <c r="P6" s="1">
+        <v>639.12</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>639.12</v>
       </c>
       <c r="R6" s="6">
         <v>45</v>
@@ -1484,10 +1498,10 @@
       <c r="S6" s="6">
         <v>65</v>
       </c>
-      <c r="T6" s="6">
+      <c r="T6" s="10">
         <v>0.375</v>
       </c>
-      <c r="U6" s="6">
+      <c r="U6" s="10">
         <v>0.6</v>
       </c>
       <c r="V6" s="6">
@@ -1499,10 +1513,10 @@
       <c r="X6" s="6">
         <v>70</v>
       </c>
-      <c r="Y6" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="6">
+      <c r="Y6" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="9">
         <v>0</v>
       </c>
       <c r="AA6" s="6">
@@ -1525,20 +1539,20 @@
       <c r="C7" s="6">
         <v>600</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="10">
         <f t="shared" si="0"/>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G7" s="6">
-        <v>0</v>
-      </c>
-      <c r="H7" s="6">
+      <c r="G7" s="10">
+        <v>0</v>
+      </c>
+      <c r="H7" s="10">
         <v>0</v>
       </c>
       <c r="I7" s="6">
@@ -1562,11 +1576,11 @@
       <c r="O7" s="6">
         <v>27.06</v>
       </c>
-      <c r="P7" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="7">
-        <v>0</v>
+      <c r="P7" s="1">
+        <v>783.96</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>783.96</v>
       </c>
       <c r="R7" s="6">
         <v>45</v>
@@ -1574,10 +1588,10 @@
       <c r="S7" s="6">
         <v>65</v>
       </c>
-      <c r="T7" s="6">
+      <c r="T7" s="10">
         <v>0.375</v>
       </c>
-      <c r="U7" s="6">
+      <c r="U7" s="10">
         <v>0.6</v>
       </c>
       <c r="V7" s="6">
@@ -1589,10 +1603,10 @@
       <c r="X7" s="6">
         <v>70</v>
       </c>
-      <c r="Y7" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="6">
+      <c r="Y7" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="9">
         <v>0</v>
       </c>
       <c r="AA7" s="6">
@@ -1615,20 +1629,20 @@
       <c r="C8" s="6">
         <v>600</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="10">
         <f t="shared" si="0"/>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G8" s="6">
-        <v>0</v>
-      </c>
-      <c r="H8" s="6">
+      <c r="G8" s="10">
+        <v>0</v>
+      </c>
+      <c r="H8" s="10">
         <v>0</v>
       </c>
       <c r="I8" s="6">
@@ -1652,11 +1666,11 @@
       <c r="O8" s="6">
         <v>27.6</v>
       </c>
-      <c r="P8" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="7">
-        <v>0</v>
+      <c r="P8" s="1">
+        <v>933.72</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>933.72</v>
       </c>
       <c r="R8" s="6">
         <v>45</v>
@@ -1664,10 +1678,10 @@
       <c r="S8" s="6">
         <v>65</v>
       </c>
-      <c r="T8" s="6">
+      <c r="T8" s="10">
         <v>0.375</v>
       </c>
-      <c r="U8" s="6">
+      <c r="U8" s="10">
         <v>0.6</v>
       </c>
       <c r="V8" s="6">
@@ -1679,10 +1693,10 @@
       <c r="X8" s="6">
         <v>70</v>
       </c>
-      <c r="Y8" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="6">
+      <c r="Y8" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="9">
         <v>0</v>
       </c>
       <c r="AA8" s="6">
@@ -1705,20 +1719,20 @@
       <c r="C9" s="6">
         <v>700</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="10">
         <f t="shared" si="0"/>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G9" s="6">
-        <v>0</v>
-      </c>
-      <c r="H9" s="6">
+      <c r="G9" s="10">
+        <v>0</v>
+      </c>
+      <c r="H9" s="10">
         <v>0</v>
       </c>
       <c r="I9" s="6">
@@ -1742,11 +1756,11 @@
       <c r="O9" s="6">
         <v>80</v>
       </c>
-      <c r="P9" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="7">
-        <v>0</v>
+      <c r="P9" s="8">
+        <v>1108.32</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>1108.32</v>
       </c>
       <c r="R9" s="6">
         <v>45</v>
@@ -1754,10 +1768,10 @@
       <c r="S9" s="6">
         <v>65</v>
       </c>
-      <c r="T9" s="6">
+      <c r="T9" s="10">
         <v>0.375</v>
       </c>
-      <c r="U9" s="6">
+      <c r="U9" s="10">
         <v>0.6</v>
       </c>
       <c r="V9" s="6">
@@ -1769,10 +1783,10 @@
       <c r="X9" s="6">
         <v>70</v>
       </c>
-      <c r="Y9" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="6">
+      <c r="Y9" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="9">
         <v>0</v>
       </c>
       <c r="AA9" s="6">
@@ -1795,20 +1809,20 @@
       <c r="C10" s="6">
         <v>700</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="10">
         <f t="shared" si="0"/>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G10" s="6">
-        <v>0</v>
-      </c>
-      <c r="H10" s="6">
+      <c r="G10" s="10">
+        <v>0</v>
+      </c>
+      <c r="H10" s="10">
         <v>0</v>
       </c>
       <c r="I10" s="6">
@@ -1832,11 +1846,11 @@
       <c r="O10" s="6">
         <v>86.56</v>
       </c>
-      <c r="P10" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="7">
-        <v>0</v>
+      <c r="P10" s="8">
+        <v>1337.52</v>
+      </c>
+      <c r="Q10" s="8">
+        <v>1337.52</v>
       </c>
       <c r="R10" s="6">
         <v>45</v>
@@ -1844,10 +1858,10 @@
       <c r="S10" s="6">
         <v>65</v>
       </c>
-      <c r="T10" s="6">
+      <c r="T10" s="10">
         <v>0.375</v>
       </c>
-      <c r="U10" s="6">
+      <c r="U10" s="10">
         <v>0.6</v>
       </c>
       <c r="V10" s="6">
@@ -1859,10 +1873,10 @@
       <c r="X10" s="6">
         <v>70</v>
       </c>
-      <c r="Y10" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="6">
+      <c r="Y10" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="9">
         <v>0</v>
       </c>
       <c r="AA10" s="6">
@@ -1885,20 +1899,20 @@
       <c r="C11" s="6">
         <v>700</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="10">
         <f t="shared" si="0"/>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G11" s="6">
-        <v>0</v>
-      </c>
-      <c r="H11" s="6">
+      <c r="G11" s="10">
+        <v>0</v>
+      </c>
+      <c r="H11" s="10">
         <v>0</v>
       </c>
       <c r="I11" s="6">
@@ -1922,11 +1936,11 @@
       <c r="O11" s="6">
         <v>95.56</v>
       </c>
-      <c r="P11" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="7">
-        <v>0</v>
+      <c r="P11" s="8">
+        <v>1644.48</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>1644.48</v>
       </c>
       <c r="R11" s="6">
         <v>45</v>
@@ -1934,10 +1948,10 @@
       <c r="S11" s="6">
         <v>65</v>
       </c>
-      <c r="T11" s="6">
+      <c r="T11" s="10">
         <v>0.375</v>
       </c>
-      <c r="U11" s="6">
+      <c r="U11" s="10">
         <v>0.6</v>
       </c>
       <c r="V11" s="6">
@@ -1949,10 +1963,10 @@
       <c r="X11" s="6">
         <v>70</v>
       </c>
-      <c r="Y11" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="6">
+      <c r="Y11" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="9">
         <v>0</v>
       </c>
       <c r="AA11" s="6">
@@ -1975,20 +1989,20 @@
       <c r="C12" s="6">
         <v>800</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="10">
         <f t="shared" si="0"/>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G12" s="6">
-        <v>0</v>
-      </c>
-      <c r="H12" s="6">
+      <c r="G12" s="10">
+        <v>0</v>
+      </c>
+      <c r="H12" s="10">
         <v>0</v>
       </c>
       <c r="I12" s="6">
@@ -2012,11 +2026,11 @@
       <c r="O12" s="6">
         <v>106.26</v>
       </c>
-      <c r="P12" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="7">
-        <v>0</v>
+      <c r="P12" s="1">
+        <v>1858.3200000000002</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>1858.3200000000002</v>
       </c>
       <c r="R12" s="6">
         <v>45</v>
@@ -2024,10 +2038,10 @@
       <c r="S12" s="6">
         <v>65</v>
       </c>
-      <c r="T12" s="6">
+      <c r="T12" s="10">
         <v>0.375</v>
       </c>
-      <c r="U12" s="6">
+      <c r="U12" s="10">
         <v>0.6</v>
       </c>
       <c r="V12" s="6">
@@ -2039,10 +2053,10 @@
       <c r="X12" s="6">
         <v>70</v>
       </c>
-      <c r="Y12" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="6">
+      <c r="Y12" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="9">
         <v>0</v>
       </c>
       <c r="AA12" s="6">
@@ -2065,20 +2079,20 @@
       <c r="C13" s="6">
         <v>900</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="10">
         <f t="shared" si="0"/>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G13" s="6">
-        <v>0</v>
-      </c>
-      <c r="H13" s="6">
+      <c r="G13" s="10">
+        <v>0</v>
+      </c>
+      <c r="H13" s="10">
         <v>0</v>
       </c>
       <c r="I13" s="6">
@@ -2102,11 +2116,11 @@
       <c r="O13" s="6">
         <v>114.96</v>
       </c>
-      <c r="P13" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="7">
-        <v>0</v>
+      <c r="P13" s="1">
+        <v>2083.3200000000002</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>2083.3200000000002</v>
       </c>
       <c r="R13" s="6">
         <v>45</v>
@@ -2114,10 +2128,10 @@
       <c r="S13" s="6">
         <v>65</v>
       </c>
-      <c r="T13" s="6">
+      <c r="T13" s="10">
         <v>0.375</v>
       </c>
-      <c r="U13" s="6">
+      <c r="U13" s="10">
         <v>0.6</v>
       </c>
       <c r="V13" s="6">
@@ -2129,10 +2143,10 @@
       <c r="X13" s="6">
         <v>70</v>
       </c>
-      <c r="Y13" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="6">
+      <c r="Y13" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="9">
         <v>0</v>
       </c>
       <c r="AA13" s="6">
@@ -2155,20 +2169,20 @@
       <c r="C14" s="6">
         <v>1000</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="10">
         <f t="shared" si="0"/>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G14" s="6">
-        <v>0</v>
-      </c>
-      <c r="H14" s="6">
+      <c r="G14" s="10">
+        <v>0</v>
+      </c>
+      <c r="H14" s="10">
         <v>0</v>
       </c>
       <c r="I14" s="6">
@@ -2192,11 +2206,11 @@
       <c r="O14" s="6">
         <v>123.56</v>
       </c>
-      <c r="P14" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="7">
-        <v>0</v>
+      <c r="P14" s="1">
+        <v>2333.2799999999997</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>2333.2799999999997</v>
       </c>
       <c r="R14" s="6">
         <v>45</v>
@@ -2204,10 +2218,10 @@
       <c r="S14" s="6">
         <v>65</v>
       </c>
-      <c r="T14" s="6">
+      <c r="T14" s="10">
         <v>0.375</v>
       </c>
-      <c r="U14" s="6">
+      <c r="U14" s="10">
         <v>0.6</v>
       </c>
       <c r="V14" s="6">
@@ -2219,10 +2233,10 @@
       <c r="X14" s="6">
         <v>70</v>
       </c>
-      <c r="Y14" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="6">
+      <c r="Y14" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="9">
         <v>0</v>
       </c>
       <c r="AA14" s="6">
@@ -2245,20 +2259,20 @@
       <c r="C15" s="6">
         <v>1100</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="10">
         <f t="shared" si="0"/>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G15" s="6">
-        <v>0</v>
-      </c>
-      <c r="H15" s="6">
+      <c r="G15" s="10">
+        <v>0</v>
+      </c>
+      <c r="H15" s="10">
         <v>0</v>
       </c>
       <c r="I15" s="6">
@@ -2282,11 +2296,11 @@
       <c r="O15" s="6">
         <v>134.63999999999999</v>
       </c>
-      <c r="P15" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="7">
-        <v>0</v>
+      <c r="P15" s="1">
+        <v>2616.7200000000003</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>2616.7200000000003</v>
       </c>
       <c r="R15" s="6">
         <v>45</v>
@@ -2294,10 +2308,10 @@
       <c r="S15" s="6">
         <v>65</v>
       </c>
-      <c r="T15" s="6">
+      <c r="T15" s="10">
         <v>0.375</v>
       </c>
-      <c r="U15" s="6">
+      <c r="U15" s="10">
         <v>0.6</v>
       </c>
       <c r="V15" s="6">
@@ -2309,10 +2323,10 @@
       <c r="X15" s="6">
         <v>70</v>
       </c>
-      <c r="Y15" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z15" s="6">
+      <c r="Y15" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="9">
         <v>0</v>
       </c>
       <c r="AA15" s="6">
@@ -2335,20 +2349,20 @@
       <c r="C16" s="6">
         <v>1300</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="10">
         <f t="shared" si="0"/>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G16" s="6">
-        <v>0</v>
-      </c>
-      <c r="H16" s="6">
+      <c r="G16" s="10">
+        <v>0</v>
+      </c>
+      <c r="H16" s="10">
         <v>0</v>
       </c>
       <c r="I16" s="6">
@@ -2372,11 +2386,11 @@
       <c r="O16" s="6">
         <v>146.78</v>
       </c>
-      <c r="P16" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="7">
-        <v>0</v>
+      <c r="P16" s="1">
+        <v>2933.28</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>2933.28</v>
       </c>
       <c r="R16" s="6">
         <v>45</v>
@@ -2384,10 +2398,10 @@
       <c r="S16" s="6">
         <v>65</v>
       </c>
-      <c r="T16" s="6">
+      <c r="T16" s="10">
         <v>0.375</v>
       </c>
-      <c r="U16" s="6">
+      <c r="U16" s="10">
         <v>0.6</v>
       </c>
       <c r="V16" s="6">
@@ -2399,10 +2413,10 @@
       <c r="X16" s="6">
         <v>70</v>
       </c>
-      <c r="Y16" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z16" s="6">
+      <c r="Y16" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="9">
         <v>0</v>
       </c>
       <c r="AA16" s="6">
@@ -2425,20 +2439,20 @@
       <c r="C17" s="6">
         <v>1400</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="10">
         <f t="shared" si="0"/>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G17" s="6">
-        <v>0</v>
-      </c>
-      <c r="H17" s="6">
+      <c r="G17" s="10">
+        <v>0</v>
+      </c>
+      <c r="H17" s="10">
         <v>0</v>
       </c>
       <c r="I17" s="6">
@@ -2462,11 +2476,11 @@
       <c r="O17" s="6">
         <v>161.31</v>
       </c>
-      <c r="P17" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="7">
-        <v>0</v>
+      <c r="P17" s="1">
+        <v>3291.72</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>3291.72</v>
       </c>
       <c r="R17" s="6">
         <v>45</v>
@@ -2474,10 +2488,10 @@
       <c r="S17" s="6">
         <v>65</v>
       </c>
-      <c r="T17" s="6">
+      <c r="T17" s="10">
         <v>0.375</v>
       </c>
-      <c r="U17" s="6">
+      <c r="U17" s="10">
         <v>0.6</v>
       </c>
       <c r="V17" s="6">
@@ -2489,10 +2503,10 @@
       <c r="X17" s="6">
         <v>70</v>
       </c>
-      <c r="Y17" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="6">
+      <c r="Y17" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="9">
         <v>0</v>
       </c>
       <c r="AA17" s="6">
@@ -2515,20 +2529,20 @@
       <c r="C18" s="6">
         <v>1600</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="10">
         <f t="shared" si="0"/>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G18" s="6">
-        <v>0</v>
-      </c>
-      <c r="H18" s="6">
+      <c r="G18" s="10">
+        <v>0</v>
+      </c>
+      <c r="H18" s="10">
         <v>0</v>
       </c>
       <c r="I18" s="6">
@@ -2552,11 +2566,11 @@
       <c r="O18" s="6">
         <v>181.18</v>
       </c>
-      <c r="P18" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="7">
-        <v>0</v>
+      <c r="P18" s="1">
+        <v>3691.8</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>3691.8</v>
       </c>
       <c r="R18" s="6">
         <v>45</v>
@@ -2564,10 +2578,10 @@
       <c r="S18" s="6">
         <v>65</v>
       </c>
-      <c r="T18" s="6">
+      <c r="T18" s="10">
         <v>0.375</v>
       </c>
-      <c r="U18" s="6">
+      <c r="U18" s="10">
         <v>0.6</v>
       </c>
       <c r="V18" s="6">
@@ -2579,10 +2593,10 @@
       <c r="X18" s="6">
         <v>70</v>
       </c>
-      <c r="Y18" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="6">
+      <c r="Y18" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="9">
         <v>0</v>
       </c>
       <c r="AA18" s="6">
@@ -2605,20 +2619,20 @@
       <c r="C19" s="6">
         <v>1800</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="10">
         <f t="shared" si="0"/>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G19" s="6">
-        <v>0</v>
-      </c>
-      <c r="H19" s="6">
+      <c r="G19" s="10">
+        <v>0</v>
+      </c>
+      <c r="H19" s="10">
         <v>0</v>
       </c>
       <c r="I19" s="6">
@@ -2642,11 +2656,11 @@
       <c r="O19" s="6">
         <v>201.44</v>
       </c>
-      <c r="P19" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="7">
-        <v>0</v>
+      <c r="P19" s="1">
+        <v>4141.8</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>4141.8</v>
       </c>
       <c r="R19" s="6">
         <v>45</v>
@@ -2654,10 +2668,10 @@
       <c r="S19" s="6">
         <v>65</v>
       </c>
-      <c r="T19" s="6">
+      <c r="T19" s="10">
         <v>0.375</v>
       </c>
-      <c r="U19" s="6">
+      <c r="U19" s="10">
         <v>0.6</v>
       </c>
       <c r="V19" s="6">
@@ -2669,10 +2683,10 @@
       <c r="X19" s="6">
         <v>70</v>
       </c>
-      <c r="Y19" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z19" s="6">
+      <c r="Y19" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="9">
         <v>0</v>
       </c>
       <c r="AA19" s="6">
@@ -2695,20 +2709,20 @@
       <c r="C20" s="6">
         <v>2000</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="10">
         <f t="shared" si="0"/>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="10">
         <v>0.06</v>
       </c>
-      <c r="H20" s="6">
+      <c r="H20" s="10">
         <v>0.06</v>
       </c>
       <c r="I20" s="6">
@@ -2732,11 +2746,11 @@
       <c r="O20" s="6">
         <v>214.94</v>
       </c>
-      <c r="P20" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="7">
-        <v>0</v>
+      <c r="P20" s="1">
+        <v>4650</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>4650</v>
       </c>
       <c r="R20" s="6">
         <v>45</v>
@@ -2744,10 +2758,10 @@
       <c r="S20" s="6">
         <v>65</v>
       </c>
-      <c r="T20" s="6">
+      <c r="T20" s="10">
         <v>0.375</v>
       </c>
-      <c r="U20" s="6">
+      <c r="U20" s="10">
         <v>0.6</v>
       </c>
       <c r="V20" s="6">
@@ -2759,10 +2773,10 @@
       <c r="X20" s="6">
         <v>70</v>
       </c>
-      <c r="Y20" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z20" s="6">
+      <c r="Y20" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="9">
         <v>0</v>
       </c>
       <c r="AA20" s="6">
@@ -2785,20 +2799,20 @@
       <c r="C21" s="6">
         <v>2300</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="10">
         <f t="shared" si="0"/>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="10">
         <v>0.06</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H21" s="10">
         <v>0.06</v>
       </c>
       <c r="I21" s="6">
@@ -2822,11 +2836,11 @@
       <c r="O21" s="6">
         <v>224.4</v>
       </c>
-      <c r="P21" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="7">
-        <v>0</v>
+      <c r="P21" s="1">
+        <v>5225.04</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>5225.04</v>
       </c>
       <c r="R21" s="6">
         <v>45</v>
@@ -2834,10 +2848,10 @@
       <c r="S21" s="6">
         <v>65</v>
       </c>
-      <c r="T21" s="6">
+      <c r="T21" s="10">
         <v>0.375</v>
       </c>
-      <c r="U21" s="6">
+      <c r="U21" s="10">
         <v>0.6</v>
       </c>
       <c r="V21" s="6">
@@ -2849,10 +2863,10 @@
       <c r="X21" s="6">
         <v>70</v>
       </c>
-      <c r="Y21" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z21" s="6">
+      <c r="Y21" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="9">
         <v>0</v>
       </c>
       <c r="AA21" s="6">
@@ -2875,20 +2889,20 @@
       <c r="C22" s="6">
         <v>2500</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="10">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="10">
         <f t="shared" si="0"/>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="10">
         <v>0.06</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H22" s="10">
         <v>0.06</v>
       </c>
       <c r="I22" s="6">
@@ -2912,11 +2926,11 @@
       <c r="O22" s="6">
         <v>233.38</v>
       </c>
-      <c r="P22" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="7">
-        <v>0</v>
+      <c r="P22" s="1">
+        <v>5833.32</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>5833.32</v>
       </c>
       <c r="R22" s="6">
         <v>45</v>
@@ -2924,10 +2938,10 @@
       <c r="S22" s="6">
         <v>65</v>
       </c>
-      <c r="T22" s="6">
+      <c r="T22" s="10">
         <v>0.375</v>
       </c>
-      <c r="U22" s="6">
+      <c r="U22" s="10">
         <v>0.6</v>
       </c>
       <c r="V22" s="6">
@@ -2939,10 +2953,10 @@
       <c r="X22" s="6">
         <v>70</v>
       </c>
-      <c r="Y22" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z22" s="6">
+      <c r="Y22" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="9">
         <v>0</v>
       </c>
       <c r="AA22" s="6">
@@ -2965,20 +2979,20 @@
       <c r="C23" s="6">
         <v>2500</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="10">
         <v>1.9E-2</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="10">
         <v>1.9E-2</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="10">
         <f t="shared" si="0"/>
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G23" s="10">
         <v>0.06</v>
       </c>
-      <c r="H23" s="6">
+      <c r="H23" s="10">
         <v>0.06</v>
       </c>
       <c r="I23" s="6">
@@ -3002,11 +3016,11 @@
       <c r="O23" s="6">
         <v>242.95</v>
       </c>
-      <c r="P23" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="7">
-        <v>0</v>
+      <c r="P23" s="1">
+        <v>6258.24</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>6258.24</v>
       </c>
       <c r="R23" s="6">
         <v>45</v>
@@ -3014,10 +3028,10 @@
       <c r="S23" s="6">
         <v>65</v>
       </c>
-      <c r="T23" s="6">
+      <c r="T23" s="10">
         <v>0.375</v>
       </c>
-      <c r="U23" s="6">
+      <c r="U23" s="10">
         <v>0.6</v>
       </c>
       <c r="V23" s="6">
@@ -3029,10 +3043,10 @@
       <c r="X23" s="6">
         <v>70</v>
       </c>
-      <c r="Y23" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z23" s="6">
+      <c r="Y23" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="9">
         <v>0</v>
       </c>
       <c r="AA23" s="6">
@@ -3055,20 +3069,20 @@
       <c r="C24" s="6">
         <v>2600</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="10">
         <v>0.02</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="10">
         <v>0.02</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="10">
         <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
-      <c r="G24" s="6">
+      <c r="G24" s="10">
         <v>0.06</v>
       </c>
-      <c r="H24" s="6">
+      <c r="H24" s="10">
         <v>0.06</v>
       </c>
       <c r="I24" s="6">
@@ -3092,11 +3106,11 @@
       <c r="O24" s="6">
         <v>253.64</v>
       </c>
-      <c r="P24" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="7">
-        <v>0</v>
+      <c r="P24" s="1">
+        <v>6516.7199999999993</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>6516.7199999999993</v>
       </c>
       <c r="R24" s="6">
         <v>45</v>
@@ -3104,10 +3118,10 @@
       <c r="S24" s="6">
         <v>65</v>
       </c>
-      <c r="T24" s="6">
+      <c r="T24" s="10">
         <v>0.375</v>
       </c>
-      <c r="U24" s="6">
+      <c r="U24" s="10">
         <v>0.6</v>
       </c>
       <c r="V24" s="6">
@@ -3119,10 +3133,10 @@
       <c r="X24" s="6">
         <v>70</v>
       </c>
-      <c r="Y24" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z24" s="6">
+      <c r="Y24" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="9">
         <v>0</v>
       </c>
       <c r="AA24" s="6">
@@ -3145,20 +3159,20 @@
       <c r="C25" s="6">
         <v>2700</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="10">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="10">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="10">
         <f t="shared" si="0"/>
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25" s="10">
         <v>0.06</v>
       </c>
-      <c r="H25" s="6">
+      <c r="H25" s="10">
         <v>0.06</v>
       </c>
       <c r="I25" s="6">
@@ -3182,11 +3196,11 @@
       <c r="O25" s="6">
         <v>264.04000000000002</v>
       </c>
-      <c r="P25" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="7">
-        <v>0</v>
+      <c r="P25" s="1">
+        <v>6675</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>6675</v>
       </c>
       <c r="R25" s="6">
         <v>45</v>
@@ -3194,10 +3208,10 @@
       <c r="S25" s="6">
         <v>65</v>
       </c>
-      <c r="T25" s="6">
+      <c r="T25" s="10">
         <v>0.375</v>
       </c>
-      <c r="U25" s="6">
+      <c r="U25" s="10">
         <v>0.6</v>
       </c>
       <c r="V25" s="6">
@@ -3209,10 +3223,10 @@
       <c r="X25" s="6">
         <v>70</v>
       </c>
-      <c r="Y25" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z25" s="6">
+      <c r="Y25" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="9">
         <v>0</v>
       </c>
       <c r="AA25" s="6">
@@ -3235,20 +3249,20 @@
       <c r="C26" s="6">
         <v>2800</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="10">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="10">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="10">
         <f t="shared" si="0"/>
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="G26" s="6">
+      <c r="G26" s="10">
         <v>0.06</v>
       </c>
-      <c r="H26" s="6">
+      <c r="H26" s="10">
         <v>0.06</v>
       </c>
       <c r="I26" s="6">
@@ -3272,11 +3286,11 @@
       <c r="O26" s="6">
         <v>276.70999999999998</v>
       </c>
-      <c r="P26" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="7">
-        <v>0</v>
+      <c r="P26" s="1">
+        <v>6924.9600000000009</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>6924.9600000000009</v>
       </c>
       <c r="R26" s="6">
         <v>45</v>
@@ -3284,10 +3298,10 @@
       <c r="S26" s="6">
         <v>65</v>
       </c>
-      <c r="T26" s="6">
+      <c r="T26" s="10">
         <v>0.375</v>
       </c>
-      <c r="U26" s="6">
+      <c r="U26" s="10">
         <v>0.6</v>
       </c>
       <c r="V26" s="6">
@@ -3299,10 +3313,10 @@
       <c r="X26" s="6">
         <v>70</v>
       </c>
-      <c r="Y26" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="Z26" s="6">
+      <c r="Y26" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="Z26" s="9">
         <v>0</v>
       </c>
       <c r="AA26" s="6">
@@ -3325,20 +3339,20 @@
       <c r="C27" s="6">
         <v>3000</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="10">
         <v>2.3E-2</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="10">
         <v>2.3E-2</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27" s="10">
         <f t="shared" si="0"/>
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="G27" s="6">
+      <c r="G27" s="10">
         <v>0.06</v>
       </c>
-      <c r="H27" s="6">
+      <c r="H27" s="10">
         <v>0.06</v>
       </c>
       <c r="I27" s="6">
@@ -3362,11 +3376,11 @@
       <c r="O27" s="6">
         <v>289.99</v>
       </c>
-      <c r="P27" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="7">
-        <v>0</v>
+      <c r="P27" s="1">
+        <v>7258.32</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>7258.32</v>
       </c>
       <c r="R27" s="6">
         <v>45</v>
@@ -3374,10 +3388,10 @@
       <c r="S27" s="6">
         <v>65</v>
       </c>
-      <c r="T27" s="6">
+      <c r="T27" s="10">
         <v>0.375</v>
       </c>
-      <c r="U27" s="6">
+      <c r="U27" s="10">
         <v>0.6</v>
       </c>
       <c r="V27" s="6">
@@ -3389,10 +3403,10 @@
       <c r="X27" s="6">
         <v>70</v>
       </c>
-      <c r="Y27" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="Z27" s="6">
+      <c r="Y27" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="Z27" s="9">
         <v>0</v>
       </c>
       <c r="AA27" s="6">
@@ -3415,20 +3429,20 @@
       <c r="C28" s="6">
         <v>3200</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="10">
         <v>2.4E-2</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="10">
         <v>2.4E-2</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F28" s="10">
         <f t="shared" si="0"/>
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="G28" s="6">
+      <c r="G28" s="10">
         <v>0.06</v>
       </c>
-      <c r="H28" s="6">
+      <c r="H28" s="10">
         <v>0.06</v>
       </c>
       <c r="I28" s="6">
@@ -3452,11 +3466,11 @@
       <c r="O28" s="6">
         <v>306.81</v>
       </c>
-      <c r="P28" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="7">
-        <v>0</v>
+      <c r="P28" s="1">
+        <v>7633.32</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>7633.32</v>
       </c>
       <c r="R28" s="6">
         <v>45</v>
@@ -3464,10 +3478,10 @@
       <c r="S28" s="6">
         <v>65</v>
       </c>
-      <c r="T28" s="6">
+      <c r="T28" s="10">
         <v>0.375</v>
       </c>
-      <c r="U28" s="6">
+      <c r="U28" s="10">
         <v>0.6</v>
       </c>
       <c r="V28" s="6">
@@ -3479,10 +3493,10 @@
       <c r="X28" s="6">
         <v>70</v>
       </c>
-      <c r="Y28" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="Z28" s="6">
+      <c r="Y28" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="Z28" s="9">
         <v>0</v>
       </c>
       <c r="AA28" s="6">
@@ -3505,20 +3519,20 @@
       <c r="C29" s="6">
         <v>3300</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="10">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="10">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F29" s="6">
+      <c r="F29" s="10">
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="G29" s="6">
+      <c r="G29" s="10">
         <v>0.06</v>
       </c>
-      <c r="H29" s="6">
+      <c r="H29" s="10">
         <v>0.06</v>
       </c>
       <c r="I29" s="6">
@@ -3542,11 +3556,11 @@
       <c r="O29" s="6">
         <v>312.33</v>
       </c>
-      <c r="P29" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="7">
-        <v>0</v>
+      <c r="P29" s="1">
+        <v>8008.32</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>8008.32</v>
       </c>
       <c r="R29" s="6">
         <v>45</v>
@@ -3554,10 +3568,10 @@
       <c r="S29" s="6">
         <v>65</v>
       </c>
-      <c r="T29" s="6">
+      <c r="T29" s="10">
         <v>0.375</v>
       </c>
-      <c r="U29" s="6">
+      <c r="U29" s="10">
         <v>0.6</v>
       </c>
       <c r="V29" s="6">
@@ -3569,10 +3583,10 @@
       <c r="X29" s="6">
         <v>70</v>
       </c>
-      <c r="Y29" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="Z29" s="6">
+      <c r="Y29" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="Z29" s="9">
         <v>0</v>
       </c>
       <c r="AA29" s="6">
@@ -3595,20 +3609,20 @@
       <c r="C30" s="6">
         <v>3400</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="10">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="10">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="F30" s="6">
+      <c r="F30" s="10">
         <f t="shared" si="0"/>
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="G30" s="6">
+      <c r="G30" s="10">
         <v>0.06</v>
       </c>
-      <c r="H30" s="6">
+      <c r="H30" s="10">
         <v>0.06</v>
       </c>
       <c r="I30" s="6">
@@ -3632,11 +3646,11 @@
       <c r="O30" s="6">
         <v>81.52</v>
       </c>
-      <c r="P30" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="7">
-        <v>0</v>
+      <c r="P30" s="1">
+        <v>8333.2800000000007</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>8333.2800000000007</v>
       </c>
       <c r="R30" s="6">
         <v>45</v>
@@ -3644,10 +3658,10 @@
       <c r="S30" s="6">
         <v>65</v>
       </c>
-      <c r="T30" s="6">
+      <c r="T30" s="10">
         <v>0.375</v>
       </c>
-      <c r="U30" s="6">
+      <c r="U30" s="10">
         <v>0.6</v>
       </c>
       <c r="V30" s="6">
@@ -3659,10 +3673,10 @@
       <c r="X30" s="6">
         <v>70</v>
       </c>
-      <c r="Y30" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="Z30" s="6">
+      <c r="Y30" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="Z30" s="9">
         <v>0</v>
       </c>
       <c r="AA30" s="6">
@@ -3685,20 +3699,20 @@
       <c r="C31" s="6">
         <v>3400</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="10">
         <v>2.7E-2</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="10">
         <v>2.7E-2</v>
       </c>
-      <c r="F31" s="6">
+      <c r="F31" s="10">
         <f t="shared" si="0"/>
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="G31" s="6">
+      <c r="G31" s="10">
         <v>0.06</v>
       </c>
-      <c r="H31" s="6">
+      <c r="H31" s="10">
         <v>0.06</v>
       </c>
       <c r="I31" s="6">
@@ -3722,11 +3736,11 @@
       <c r="O31" s="6">
         <v>81.52</v>
       </c>
-      <c r="P31" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="7">
-        <v>0</v>
+      <c r="P31" s="1">
+        <v>8558.2800000000007</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>8558.2800000000007</v>
       </c>
       <c r="R31" s="6">
         <v>45</v>
@@ -3734,10 +3748,10 @@
       <c r="S31" s="6">
         <v>65</v>
       </c>
-      <c r="T31" s="6">
+      <c r="T31" s="10">
         <v>0.375</v>
       </c>
-      <c r="U31" s="6">
+      <c r="U31" s="10">
         <v>0.6</v>
       </c>
       <c r="V31" s="6">
@@ -3749,10 +3763,10 @@
       <c r="X31" s="6">
         <v>70</v>
       </c>
-      <c r="Y31" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="Z31" s="6">
+      <c r="Y31" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="Z31" s="9">
         <v>0</v>
       </c>
       <c r="AA31" s="6">
@@ -3775,20 +3789,20 @@
       <c r="C32" s="6">
         <v>3500</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="10">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="10">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="F32" s="6">
+      <c r="F32" s="10">
         <f t="shared" si="0"/>
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="G32" s="6">
+      <c r="G32" s="10">
         <v>0.06</v>
       </c>
-      <c r="H32" s="6">
+      <c r="H32" s="10">
         <v>0.06</v>
       </c>
       <c r="I32" s="6">
@@ -3812,11 +3826,11 @@
       <c r="O32" s="6">
         <v>83.39</v>
       </c>
-      <c r="P32" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q32" s="7">
-        <v>0</v>
+      <c r="P32" s="1">
+        <v>8724.9600000000009</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>8724.9600000000009</v>
       </c>
       <c r="R32" s="6">
         <v>45</v>
@@ -3824,10 +3838,10 @@
       <c r="S32" s="6">
         <v>65</v>
       </c>
-      <c r="T32" s="6">
+      <c r="T32" s="10">
         <v>0.375</v>
       </c>
-      <c r="U32" s="6">
+      <c r="U32" s="10">
         <v>0.6</v>
       </c>
       <c r="V32" s="6">
@@ -3839,10 +3853,10 @@
       <c r="X32" s="6">
         <v>70</v>
       </c>
-      <c r="Y32" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="Z32" s="6">
+      <c r="Y32" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="Z32" s="9">
         <v>0</v>
       </c>
       <c r="AA32" s="6">
@@ -3865,20 +3879,20 @@
       <c r="C33" s="6">
         <v>3500</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33" s="10">
         <v>0.03</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E33" s="10">
         <v>0.03</v>
       </c>
-      <c r="F33" s="6">
+      <c r="F33" s="10">
         <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
-      <c r="G33" s="6">
+      <c r="G33" s="10">
         <v>0.06</v>
       </c>
-      <c r="H33" s="6">
+      <c r="H33" s="10">
         <v>0.06</v>
       </c>
       <c r="I33" s="6">
@@ -3902,11 +3916,11 @@
       <c r="O33" s="6">
         <v>84.64</v>
       </c>
-      <c r="P33" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q33" s="7">
-        <v>0</v>
+      <c r="P33" s="1">
+        <v>8841.7199999999993</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>8841.7199999999993</v>
       </c>
       <c r="R33" s="6">
         <v>45</v>
@@ -3914,10 +3928,10 @@
       <c r="S33" s="6">
         <v>65</v>
       </c>
-      <c r="T33" s="6">
+      <c r="T33" s="10">
         <v>0.375</v>
       </c>
-      <c r="U33" s="6">
+      <c r="U33" s="10">
         <v>0.6</v>
       </c>
       <c r="V33" s="6">
@@ -3929,10 +3943,10 @@
       <c r="X33" s="6">
         <v>70</v>
       </c>
-      <c r="Y33" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="Z33" s="6">
+      <c r="Y33" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="Z33" s="9">
         <v>0</v>
       </c>
       <c r="AA33" s="6">
@@ -3955,20 +3969,20 @@
       <c r="C34" s="6">
         <v>3500</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="10">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E34" s="10">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="F34" s="6">
+      <c r="F34" s="10">
         <f t="shared" si="0"/>
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="G34" s="6">
+      <c r="G34" s="10">
         <v>0.06</v>
       </c>
-      <c r="H34" s="6">
+      <c r="H34" s="10">
         <v>0.06</v>
       </c>
       <c r="I34" s="6">
@@ -3992,11 +4006,11 @@
       <c r="O34" s="6">
         <v>86.25</v>
       </c>
-      <c r="P34" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q34" s="7">
-        <v>0</v>
+      <c r="P34" s="1">
+        <v>8937.48</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>8937.48</v>
       </c>
       <c r="R34" s="6">
         <v>45</v>
@@ -4004,10 +4018,10 @@
       <c r="S34" s="6">
         <v>65</v>
       </c>
-      <c r="T34" s="6">
+      <c r="T34" s="10">
         <v>0.375</v>
       </c>
-      <c r="U34" s="6">
+      <c r="U34" s="10">
         <v>0.6</v>
       </c>
       <c r="V34" s="6">
@@ -4019,10 +4033,10 @@
       <c r="X34" s="6">
         <v>70</v>
       </c>
-      <c r="Y34" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="Z34" s="6">
+      <c r="Y34" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="Z34" s="9">
         <v>0</v>
       </c>
       <c r="AA34" s="6">
@@ -4045,20 +4059,20 @@
       <c r="C35" s="6">
         <v>3500</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="10">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="10">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="F35" s="6">
+      <c r="F35" s="10">
         <f t="shared" si="0"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G35" s="6">
+      <c r="G35" s="10">
         <v>0.06</v>
       </c>
-      <c r="H35" s="6">
+      <c r="H35" s="10">
         <v>0.06</v>
       </c>
       <c r="I35" s="6">
@@ -4082,11 +4096,11 @@
       <c r="O35" s="6">
         <v>87.03</v>
       </c>
-      <c r="P35" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q35" s="7">
-        <v>0</v>
+      <c r="P35" s="1">
+        <v>9020.0399999999991</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>9020.0399999999991</v>
       </c>
       <c r="R35" s="6">
         <v>45</v>
@@ -4094,10 +4108,10 @@
       <c r="S35" s="6">
         <v>65</v>
       </c>
-      <c r="T35" s="6">
+      <c r="T35" s="10">
         <v>0.375</v>
       </c>
-      <c r="U35" s="6">
+      <c r="U35" s="10">
         <v>0.6</v>
       </c>
       <c r="V35" s="6">
@@ -4109,10 +4123,10 @@
       <c r="X35" s="6">
         <v>70</v>
       </c>
-      <c r="Y35" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="Z35" s="6">
+      <c r="Y35" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="Z35" s="9">
         <v>0</v>
       </c>
       <c r="AA35" s="6">
@@ -4135,20 +4149,20 @@
       <c r="C36" s="6">
         <v>3500</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36" s="10">
         <v>3.9E-2</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E36" s="10">
         <v>3.9E-2</v>
       </c>
-      <c r="F36" s="6">
+      <c r="F36" s="10">
         <f t="shared" si="0"/>
         <v>7.8E-2</v>
       </c>
-      <c r="G36" s="6">
+      <c r="G36" s="10">
         <v>0.06</v>
       </c>
-      <c r="H36" s="6">
+      <c r="H36" s="10">
         <v>0.06</v>
       </c>
       <c r="I36" s="6">
@@ -4172,11 +4186,11 @@
       <c r="O36" s="6">
         <v>88.42</v>
       </c>
-      <c r="P36" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q36" s="7">
-        <v>0</v>
+      <c r="P36" s="1">
+        <v>9155.0399999999991</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>9155.0399999999991</v>
       </c>
       <c r="R36" s="6">
         <v>45</v>
@@ -4184,10 +4198,10 @@
       <c r="S36" s="6">
         <v>65</v>
       </c>
-      <c r="T36" s="6">
+      <c r="T36" s="10">
         <v>0.375</v>
       </c>
-      <c r="U36" s="6">
+      <c r="U36" s="10">
         <v>0.6</v>
       </c>
       <c r="V36" s="6">
@@ -4199,10 +4213,10 @@
       <c r="X36" s="6">
         <v>70</v>
       </c>
-      <c r="Y36" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="Z36" s="6">
+      <c r="Y36" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="Z36" s="9">
         <v>0</v>
       </c>
       <c r="AA36" s="6">
@@ -4225,20 +4239,20 @@
       <c r="C37" s="6">
         <v>3500</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D37" s="10">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E37" s="10">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="F37" s="6">
+      <c r="F37" s="10">
         <f t="shared" si="0"/>
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="G37" s="6">
+      <c r="G37" s="10">
         <v>0.06</v>
       </c>
-      <c r="H37" s="6">
+      <c r="H37" s="10">
         <v>0.06</v>
       </c>
       <c r="I37" s="6">
@@ -4262,11 +4276,11 @@
       <c r="O37" s="6">
         <v>90.63</v>
       </c>
-      <c r="P37" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q37" s="7">
-        <v>0</v>
+      <c r="P37" s="1">
+        <v>9300</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>9300</v>
       </c>
       <c r="R37" s="6">
         <v>45</v>
@@ -4274,10 +4288,10 @@
       <c r="S37" s="6">
         <v>65</v>
       </c>
-      <c r="T37" s="6">
+      <c r="T37" s="10">
         <v>0.375</v>
       </c>
-      <c r="U37" s="6">
+      <c r="U37" s="10">
         <v>0.6</v>
       </c>
       <c r="V37" s="6">
@@ -4289,10 +4303,10 @@
       <c r="X37" s="6">
         <v>70</v>
       </c>
-      <c r="Y37" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="Z37" s="6">
+      <c r="Y37" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="Z37" s="9">
         <v>0</v>
       </c>
       <c r="AA37" s="6">
@@ -4315,20 +4329,20 @@
       <c r="C38" s="6">
         <v>3500</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D38" s="10">
         <v>4.7E-2</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E38" s="10">
         <v>4.7E-2</v>
       </c>
-      <c r="F38" s="6">
+      <c r="F38" s="10">
         <f t="shared" si="0"/>
         <v>9.4E-2</v>
       </c>
-      <c r="G38" s="6">
+      <c r="G38" s="10">
         <v>0.06</v>
       </c>
-      <c r="H38" s="6">
+      <c r="H38" s="10">
         <v>0.06</v>
       </c>
       <c r="I38" s="6">
@@ -4352,11 +4366,11 @@
       <c r="O38" s="6">
         <v>93.35</v>
       </c>
-      <c r="P38" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q38" s="7">
-        <v>0</v>
+      <c r="P38" s="1">
+        <v>9465</v>
+      </c>
+      <c r="Q38" s="1">
+        <v>9465</v>
       </c>
       <c r="R38" s="6">
         <v>45</v>
@@ -4364,10 +4378,10 @@
       <c r="S38" s="6">
         <v>65</v>
       </c>
-      <c r="T38" s="6">
+      <c r="T38" s="10">
         <v>0.375</v>
       </c>
-      <c r="U38" s="6">
+      <c r="U38" s="10">
         <v>0.6</v>
       </c>
       <c r="V38" s="6">
@@ -4379,10 +4393,10 @@
       <c r="X38" s="6">
         <v>70</v>
       </c>
-      <c r="Y38" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="Z38" s="6">
+      <c r="Y38" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="Z38" s="9">
         <v>0</v>
       </c>
       <c r="AA38" s="6">
@@ -4405,20 +4419,20 @@
       <c r="C39" s="6">
         <v>3500</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D39" s="10">
         <v>4.9500000000000002E-2</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E39" s="10">
         <v>4.9500000000000002E-2</v>
       </c>
-      <c r="F39" s="6">
+      <c r="F39" s="10">
         <f t="shared" si="0"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="G39" s="6">
+      <c r="G39" s="10">
         <v>0.06</v>
       </c>
-      <c r="H39" s="6">
+      <c r="H39" s="10">
         <v>0.06</v>
       </c>
       <c r="I39" s="6">
@@ -4442,11 +4456,11 @@
       <c r="O39" s="6">
         <v>94.84</v>
       </c>
-      <c r="P39" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q39" s="7">
-        <v>0</v>
+      <c r="P39" s="1">
+        <v>9615</v>
+      </c>
+      <c r="Q39" s="1">
+        <v>9615</v>
       </c>
       <c r="R39" s="6">
         <v>45</v>
@@ -4454,10 +4468,10 @@
       <c r="S39" s="6">
         <v>65</v>
       </c>
-      <c r="T39" s="6">
+      <c r="T39" s="10">
         <v>0.375</v>
       </c>
-      <c r="U39" s="6">
+      <c r="U39" s="10">
         <v>0.6</v>
       </c>
       <c r="V39" s="6">
@@ -4469,10 +4483,10 @@
       <c r="X39" s="6">
         <v>70</v>
       </c>
-      <c r="Y39" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="Z39" s="6">
+      <c r="Y39" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="Z39" s="9">
         <v>0</v>
       </c>
       <c r="AA39" s="6">
@@ -4495,20 +4509,20 @@
       <c r="C40" s="6">
         <v>3500</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D40" s="10">
         <v>4.9500000000000002E-2</v>
       </c>
-      <c r="E40" s="6">
+      <c r="E40" s="10">
         <v>4.9500000000000002E-2</v>
       </c>
-      <c r="F40" s="6">
+      <c r="F40" s="10">
         <f t="shared" si="0"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="G40" s="6">
+      <c r="G40" s="10">
         <v>0.06</v>
       </c>
-      <c r="H40" s="6">
+      <c r="H40" s="10">
         <v>0.06</v>
       </c>
       <c r="I40" s="6">
@@ -4532,11 +4546,11 @@
       <c r="O40" s="6">
         <v>97.87</v>
       </c>
-      <c r="P40" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q40" s="7">
-        <v>0</v>
+      <c r="P40" s="5">
+        <v>9770.0400000000009</v>
+      </c>
+      <c r="Q40" s="5">
+        <v>9770.0400000000009</v>
       </c>
       <c r="R40" s="6">
         <v>45</v>
@@ -4544,10 +4558,10 @@
       <c r="S40" s="6">
         <v>65</v>
       </c>
-      <c r="T40" s="6">
+      <c r="T40" s="10">
         <v>0.375</v>
       </c>
-      <c r="U40" s="6">
+      <c r="U40" s="10">
         <v>0.6</v>
       </c>
       <c r="V40" s="6">
@@ -4559,10 +4573,10 @@
       <c r="X40" s="6">
         <v>70</v>
       </c>
-      <c r="Y40" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="Z40" s="6">
+      <c r="Y40" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="Z40" s="9">
         <v>0</v>
       </c>
       <c r="AA40" s="6">
@@ -4585,20 +4599,20 @@
       <c r="C41" s="6">
         <v>3500</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D41" s="10">
         <v>4.9500000000000002E-2</v>
       </c>
-      <c r="E41" s="6">
+      <c r="E41" s="10">
         <v>4.9500000000000002E-2</v>
       </c>
-      <c r="F41" s="6">
+      <c r="F41" s="10">
         <f t="shared" si="0"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="G41" s="6">
+      <c r="G41" s="10">
         <v>0.06</v>
       </c>
-      <c r="H41" s="6">
+      <c r="H41" s="10">
         <v>0.06</v>
       </c>
       <c r="I41" s="6">
@@ -4622,11 +4636,11 @@
       <c r="O41" s="6">
         <v>99.53</v>
       </c>
-      <c r="P41" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q41" s="7">
-        <v>0</v>
+      <c r="P41" s="5">
+        <v>9945</v>
+      </c>
+      <c r="Q41" s="5">
+        <v>9945</v>
       </c>
       <c r="R41" s="6">
         <v>45</v>
@@ -4634,10 +4648,10 @@
       <c r="S41" s="6">
         <v>65</v>
       </c>
-      <c r="T41" s="6">
+      <c r="T41" s="10">
         <v>0.375</v>
       </c>
-      <c r="U41" s="6">
+      <c r="U41" s="10">
         <v>0.6</v>
       </c>
       <c r="V41" s="6">
@@ -4649,10 +4663,10 @@
       <c r="X41" s="6">
         <v>70</v>
       </c>
-      <c r="Y41" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="Z41" s="6">
+      <c r="Y41" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="Z41" s="9">
         <v>0</v>
       </c>
       <c r="AA41" s="6">
@@ -4675,20 +4689,20 @@
       <c r="C42" s="6">
         <v>3500</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D42" s="10">
         <v>4.9500000000000002E-2</v>
       </c>
-      <c r="E42" s="6">
+      <c r="E42" s="10">
         <v>4.9500000000000002E-2</v>
       </c>
-      <c r="F42" s="6">
+      <c r="F42" s="10">
         <f t="shared" si="0"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="G42" s="6">
+      <c r="G42" s="10">
         <v>0.06</v>
       </c>
-      <c r="H42" s="6">
+      <c r="H42" s="10">
         <v>0.06</v>
       </c>
       <c r="I42" s="6">
@@ -4712,11 +4726,11 @@
       <c r="O42" s="6">
         <v>101.82</v>
       </c>
-      <c r="P42" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q42" s="7">
-        <v>0</v>
+      <c r="P42" s="5">
+        <v>10134.959999999999</v>
+      </c>
+      <c r="Q42" s="5">
+        <v>10134.959999999999</v>
       </c>
       <c r="R42" s="6">
         <v>45</v>
@@ -4724,10 +4738,10 @@
       <c r="S42" s="6">
         <v>65</v>
       </c>
-      <c r="T42" s="6">
+      <c r="T42" s="10">
         <v>0.375</v>
       </c>
-      <c r="U42" s="6">
+      <c r="U42" s="10">
         <v>0.6</v>
       </c>
       <c r="V42" s="6">
@@ -4739,10 +4753,10 @@
       <c r="X42" s="6">
         <v>70</v>
       </c>
-      <c r="Y42" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="Z42" s="6">
+      <c r="Y42" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="Z42" s="9">
         <v>0</v>
       </c>
       <c r="AA42" s="6">
@@ -4765,20 +4779,20 @@
       <c r="C43" s="6">
         <v>3500</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D43" s="10">
         <v>4.9500000000000002E-2</v>
       </c>
-      <c r="E43" s="6">
+      <c r="E43" s="10">
         <v>4.9500000000000002E-2</v>
       </c>
-      <c r="F43" s="6">
+      <c r="F43" s="10">
         <f t="shared" si="0"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="G43" s="6">
+      <c r="G43" s="10">
         <v>0.06</v>
       </c>
-      <c r="H43" s="6">
+      <c r="H43" s="10">
         <v>0.06</v>
       </c>
       <c r="I43" s="6">
@@ -4814,10 +4828,10 @@
       <c r="S43" s="6">
         <v>65</v>
       </c>
-      <c r="T43" s="6">
+      <c r="T43" s="10">
         <v>0.375</v>
       </c>
-      <c r="U43" s="6">
+      <c r="U43" s="10">
         <v>0.6</v>
       </c>
       <c r="V43" s="6">
@@ -4829,10 +4843,10 @@
       <c r="X43" s="6">
         <v>70</v>
       </c>
-      <c r="Y43" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="Z43" s="6">
+      <c r="Y43" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="Z43" s="9">
         <v>0</v>
       </c>
       <c r="AA43" s="6">
@@ -4855,20 +4869,20 @@
       <c r="C44" s="6">
         <v>3500</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D44" s="10">
         <v>4.9500000000000002E-2</v>
       </c>
-      <c r="E44" s="6">
+      <c r="E44" s="10">
         <v>4.9500000000000002E-2</v>
       </c>
-      <c r="F44" s="6">
+      <c r="F44" s="10">
         <f t="shared" si="0"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="G44" s="6">
+      <c r="G44" s="10">
         <v>0.06</v>
       </c>
-      <c r="H44" s="6">
+      <c r="H44" s="10">
         <v>0.06</v>
       </c>
       <c r="I44" s="6">
@@ -4904,10 +4918,10 @@
       <c r="S44" s="6">
         <v>65</v>
       </c>
-      <c r="T44" s="6">
+      <c r="T44" s="10">
         <v>0.375</v>
       </c>
-      <c r="U44" s="6">
+      <c r="U44" s="10">
         <v>0.6</v>
       </c>
       <c r="V44" s="6">
@@ -4919,10 +4933,10 @@
       <c r="X44" s="6">
         <v>70</v>
       </c>
-      <c r="Y44" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="Z44" s="6">
+      <c r="Y44" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="Z44" s="9">
         <v>0</v>
       </c>
       <c r="AA44" s="6">
@@ -4945,20 +4959,20 @@
       <c r="C45" s="6">
         <v>3500</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D45" s="10">
         <v>4.9500000000000002E-2</v>
       </c>
-      <c r="E45" s="6">
+      <c r="E45" s="10">
         <v>4.9500000000000002E-2</v>
       </c>
-      <c r="F45" s="6">
+      <c r="F45" s="10">
         <f t="shared" si="0"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="G45" s="6">
+      <c r="G45" s="10">
         <v>0.06</v>
       </c>
-      <c r="H45" s="6">
+      <c r="H45" s="10">
         <v>0.06</v>
       </c>
       <c r="I45" s="6">
@@ -4994,10 +5008,10 @@
       <c r="S45" s="6">
         <v>65</v>
       </c>
-      <c r="T45" s="6">
+      <c r="T45" s="10">
         <v>0.375</v>
       </c>
-      <c r="U45" s="6">
+      <c r="U45" s="10">
         <v>0.6</v>
       </c>
       <c r="V45" s="6">
@@ -5009,10 +5023,10 @@
       <c r="X45" s="6">
         <v>70</v>
       </c>
-      <c r="Y45" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="Z45" s="6">
+      <c r="Y45" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="Z45" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AA45" s="6">
@@ -5035,20 +5049,20 @@
       <c r="C46" s="6">
         <v>3500</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D46" s="10">
         <v>4.9500000000000002E-2</v>
       </c>
-      <c r="E46" s="6">
+      <c r="E46" s="10">
         <v>4.9500000000000002E-2</v>
       </c>
-      <c r="F46" s="6">
+      <c r="F46" s="10">
         <f t="shared" si="0"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="G46" s="6">
+      <c r="G46" s="10">
         <v>0.06</v>
       </c>
-      <c r="H46" s="6">
+      <c r="H46" s="10">
         <v>0.06</v>
       </c>
       <c r="I46" s="6">
@@ -5084,10 +5098,10 @@
       <c r="S46" s="6">
         <v>65</v>
       </c>
-      <c r="T46" s="6">
+      <c r="T46" s="10">
         <v>0.375</v>
       </c>
-      <c r="U46" s="6">
+      <c r="U46" s="10">
         <v>0.6</v>
       </c>
       <c r="V46" s="6">
@@ -5099,10 +5113,10 @@
       <c r="X46" s="6">
         <v>70</v>
       </c>
-      <c r="Y46" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="Z46" s="6">
+      <c r="Y46" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="Z46" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AA46" s="6">
@@ -5125,20 +5139,20 @@
       <c r="C47" s="6">
         <v>3500</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D47" s="10">
         <v>4.9500000000000002E-2</v>
       </c>
-      <c r="E47" s="6">
+      <c r="E47" s="10">
         <v>4.9500000000000002E-2</v>
       </c>
-      <c r="F47" s="6">
+      <c r="F47" s="10">
         <f t="shared" si="0"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="G47" s="6">
+      <c r="G47" s="10">
         <v>0.06</v>
       </c>
-      <c r="H47" s="6">
+      <c r="H47" s="10">
         <v>0.06</v>
       </c>
       <c r="I47" s="6">
@@ -5174,10 +5188,10 @@
       <c r="S47" s="6">
         <v>65</v>
       </c>
-      <c r="T47" s="6">
+      <c r="T47" s="10">
         <v>0.375</v>
       </c>
-      <c r="U47" s="6">
+      <c r="U47" s="10">
         <v>0.6</v>
       </c>
       <c r="V47" s="6">
@@ -5189,10 +5203,10 @@
       <c r="X47" s="6">
         <v>70</v>
       </c>
-      <c r="Y47" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="Z47" s="6">
+      <c r="Y47" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="Z47" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AA47" s="6">
@@ -5215,20 +5229,20 @@
       <c r="C48" s="6">
         <v>3500</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D48" s="10">
         <v>5.0250000000000003E-2</v>
       </c>
-      <c r="E48" s="6">
+      <c r="E48" s="10">
         <v>5.0250000000000003E-2</v>
       </c>
-      <c r="F48" s="6">
+      <c r="F48" s="10">
         <f t="shared" si="0"/>
         <v>0.10050000000000001</v>
       </c>
-      <c r="G48" s="6">
+      <c r="G48" s="10">
         <v>0.06</v>
       </c>
-      <c r="H48" s="6">
+      <c r="H48" s="10">
         <v>0.06</v>
       </c>
       <c r="I48" s="6">
@@ -5264,10 +5278,10 @@
       <c r="S48" s="6">
         <v>65</v>
       </c>
-      <c r="T48" s="6">
+      <c r="T48" s="10">
         <v>0.375</v>
       </c>
-      <c r="U48" s="6">
+      <c r="U48" s="10">
         <v>0.6</v>
       </c>
       <c r="V48" s="6">
@@ -5279,10 +5293,10 @@
       <c r="X48" s="6">
         <v>70</v>
       </c>
-      <c r="Y48" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="Z48" s="6">
+      <c r="Y48" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="Z48" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AA48" s="6">
@@ -5305,20 +5319,20 @@
       <c r="C49" s="6">
         <v>3500</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D49" s="10">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="E49" s="6">
+      <c r="E49" s="10">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="F49" s="6">
+      <c r="F49" s="10">
         <f t="shared" si="0"/>
         <v>0.10199999999999999</v>
       </c>
-      <c r="G49" s="6">
+      <c r="G49" s="10">
         <v>0.06</v>
       </c>
-      <c r="H49" s="6">
+      <c r="H49" s="10">
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="I49" s="6">
@@ -5354,10 +5368,10 @@
       <c r="S49" s="6">
         <v>65</v>
       </c>
-      <c r="T49" s="6">
+      <c r="T49" s="10">
         <v>0.375</v>
       </c>
-      <c r="U49" s="6">
+      <c r="U49" s="10">
         <v>0.6</v>
       </c>
       <c r="V49" s="6">
@@ -5369,10 +5383,10 @@
       <c r="X49" s="6">
         <v>70</v>
       </c>
-      <c r="Y49" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="Z49" s="6">
+      <c r="Y49" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="Z49" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AA49" s="6">
@@ -5395,20 +5409,20 @@
       <c r="C50" s="6">
         <v>3500</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D50" s="10">
         <v>5.1749999999999997E-2</v>
       </c>
-      <c r="E50" s="6">
+      <c r="E50" s="10">
         <v>5.1749999999999997E-2</v>
       </c>
-      <c r="F50" s="6">
+      <c r="F50" s="10">
         <f t="shared" si="0"/>
         <v>0.10349999999999999</v>
       </c>
-      <c r="G50" s="6">
+      <c r="G50" s="10">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="H50" s="6">
+      <c r="H50" s="10">
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="I50" s="6">
@@ -5444,10 +5458,10 @@
       <c r="S50" s="6">
         <v>65</v>
       </c>
-      <c r="T50" s="6">
+      <c r="T50" s="10">
         <v>0.375</v>
       </c>
-      <c r="U50" s="6">
+      <c r="U50" s="10">
         <v>0.6</v>
       </c>
       <c r="V50" s="6">
@@ -5459,10 +5473,10 @@
       <c r="X50" s="6">
         <v>70</v>
       </c>
-      <c r="Y50" s="6">
+      <c r="Y50" s="9">
         <v>100</v>
       </c>
-      <c r="Z50" s="6">
+      <c r="Z50" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AA50" s="6">
@@ -5485,20 +5499,20 @@
       <c r="C51" s="6">
         <v>3500</v>
       </c>
-      <c r="D51" s="6">
+      <c r="D51" s="10">
         <v>5.2499999999999998E-2</v>
       </c>
-      <c r="E51" s="6">
+      <c r="E51" s="10">
         <v>5.2499999999999998E-2</v>
       </c>
-      <c r="F51" s="6">
+      <c r="F51" s="10">
         <f t="shared" si="0"/>
         <v>0.105</v>
       </c>
-      <c r="G51" s="6">
+      <c r="G51" s="10">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="H51" s="6">
+      <c r="H51" s="10">
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="I51" s="6">
@@ -5534,10 +5548,10 @@
       <c r="S51" s="6">
         <v>65</v>
       </c>
-      <c r="T51" s="6">
+      <c r="T51" s="10">
         <v>0.375</v>
       </c>
-      <c r="U51" s="6">
+      <c r="U51" s="10">
         <v>0.6</v>
       </c>
       <c r="V51" s="6">
@@ -5549,10 +5563,10 @@
       <c r="X51" s="6">
         <v>70</v>
       </c>
-      <c r="Y51" s="6">
+      <c r="Y51" s="9">
         <v>100</v>
       </c>
-      <c r="Z51" s="6">
+      <c r="Z51" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AA51" s="6">
@@ -5575,20 +5589,20 @@
       <c r="C52" s="6">
         <v>3500</v>
       </c>
-      <c r="D52" s="6">
+      <c r="D52" s="10">
         <v>5.3249999999999999E-2</v>
       </c>
-      <c r="E52" s="6">
+      <c r="E52" s="10">
         <v>5.3249999999999999E-2</v>
       </c>
-      <c r="F52" s="6">
+      <c r="F52" s="10">
         <f t="shared" si="0"/>
         <v>0.1065</v>
       </c>
-      <c r="G52" s="6">
+      <c r="G52" s="10">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="H52" s="6">
+      <c r="H52" s="10">
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="I52" s="6">
@@ -5613,10 +5627,10 @@
         <v>120.73</v>
       </c>
       <c r="P52" s="7">
-        <v>12907.8</v>
+        <v>13110</v>
       </c>
       <c r="Q52" s="7">
-        <v>12907.8</v>
+        <v>13110</v>
       </c>
       <c r="R52" s="6">
         <v>45</v>
@@ -5624,10 +5638,10 @@
       <c r="S52" s="6">
         <v>65</v>
       </c>
-      <c r="T52" s="6">
+      <c r="T52" s="10">
         <v>0.375</v>
       </c>
-      <c r="U52" s="6">
+      <c r="U52" s="10">
         <v>0.6</v>
       </c>
       <c r="V52" s="6">
@@ -5639,10 +5653,10 @@
       <c r="X52" s="6">
         <v>70</v>
       </c>
-      <c r="Y52" s="6">
+      <c r="Y52" s="9">
         <v>100</v>
       </c>
-      <c r="Z52" s="6">
+      <c r="Z52" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AA52" s="6">
@@ -5665,20 +5679,20 @@
       <c r="C53" s="6">
         <v>3500</v>
       </c>
-      <c r="D53" s="6">
+      <c r="D53" s="10">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="E53" s="6">
+      <c r="E53" s="10">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="F53" s="6">
+      <c r="F53" s="10">
         <f t="shared" si="0"/>
         <v>0.108</v>
       </c>
-      <c r="G53" s="6">
+      <c r="G53" s="10">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="H53" s="6">
+      <c r="H53" s="10">
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="I53" s="6">
@@ -5703,10 +5717,10 @@
         <v>122.42</v>
       </c>
       <c r="P53" s="7">
-        <v>13036.88</v>
+        <v>13370.04</v>
       </c>
       <c r="Q53" s="7">
-        <v>13036.88</v>
+        <v>13370.04</v>
       </c>
       <c r="R53" s="6">
         <v>45</v>
@@ -5714,10 +5728,10 @@
       <c r="S53" s="6">
         <v>65</v>
       </c>
-      <c r="T53" s="6">
+      <c r="T53" s="10">
         <v>0.375</v>
       </c>
-      <c r="U53" s="6">
+      <c r="U53" s="10">
         <v>0.6</v>
       </c>
       <c r="V53" s="6">
@@ -5729,10 +5743,10 @@
       <c r="X53" s="6">
         <v>70</v>
       </c>
-      <c r="Y53" s="6">
+      <c r="Y53" s="9">
         <v>100</v>
       </c>
-      <c r="Z53" s="6">
+      <c r="Z53" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AA53" s="6">
@@ -5755,20 +5769,20 @@
       <c r="C54" s="6">
         <v>3500</v>
       </c>
-      <c r="D54" s="6">
+      <c r="D54" s="10">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="E54" s="6">
+      <c r="E54" s="10">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="F54" s="6">
+      <c r="F54" s="10">
         <f t="shared" si="0"/>
         <v>0.108</v>
       </c>
-      <c r="G54" s="6">
+      <c r="G54" s="10">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="H54" s="6">
+      <c r="H54" s="10">
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="I54" s="6">
@@ -5793,10 +5807,10 @@
         <v>124.26</v>
       </c>
       <c r="P54" s="7">
-        <v>13167.25</v>
+        <v>13610.04</v>
       </c>
       <c r="Q54" s="7">
-        <v>13167.25</v>
+        <v>13610.04</v>
       </c>
       <c r="R54" s="6">
         <v>45</v>
@@ -5804,10 +5818,10 @@
       <c r="S54" s="6">
         <v>65</v>
       </c>
-      <c r="T54" s="6">
+      <c r="T54" s="10">
         <v>0.375</v>
       </c>
-      <c r="U54" s="6">
+      <c r="U54" s="10">
         <v>0.6</v>
       </c>
       <c r="V54" s="6">
@@ -5819,10 +5833,10 @@
       <c r="X54" s="6">
         <v>70</v>
       </c>
-      <c r="Y54" s="6">
+      <c r="Y54" s="9">
         <v>100</v>
       </c>
-      <c r="Z54" s="6">
+      <c r="Z54" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="AA54" s="6">

</xml_diff>

<commit_message>
Add the CA column in qpp_history.xlsx
</commit_message>
<xml_diff>
--- a/params/qpp_history.xlsx
+++ b/params/qpp_history.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/UQAM/git/cpp/params/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/UQAM/Dropbox (CEDIA)/projets/claim/paper/codes/cpp/params/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="52080" yWindow="2860" windowWidth="38400" windowHeight="21140"/>
+    <workbookView xWindow="51200" yWindow="1160" windowWidth="38400" windowHeight="21140"/>
   </bookViews>
   <sheets>
     <sheet name="qppyear" sheetId="1" r:id="rId1"/>
@@ -1031,10 +1031,10 @@
   <dimension ref="A1:AM61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G55" sqref="G55:G61"/>
+      <selection pane="bottomRight" activeCell="AB67" sqref="AB67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7608,7 +7608,7 @@
       <c r="AC55" s="11">
         <v>496.36</v>
       </c>
-      <c r="AD55" s="11">
+      <c r="AD55" s="17">
         <v>2.3E-2</v>
       </c>
       <c r="AE55" s="12">
@@ -7644,8 +7644,8 @@
         <v>2020</v>
       </c>
       <c r="B56" s="11">
-        <f>B55*1.03</f>
-        <v>59122</v>
+        <f>B55*1.0159</f>
+        <v>58312.66</v>
       </c>
       <c r="C56" s="11">
         <v>3500</v>
@@ -7731,8 +7731,8 @@
         <f>AC55*1.03</f>
         <v>511.25080000000003</v>
       </c>
-      <c r="AD56" s="11">
-        <v>2.3E-2</v>
+      <c r="AD56" s="17">
+        <v>1.5900000000000001E-2</v>
       </c>
       <c r="AE56" s="12">
         <v>1</v>
@@ -7767,8 +7767,8 @@
         <v>2021</v>
       </c>
       <c r="B57" s="11">
-        <f t="shared" ref="B57:B61" si="2">B56*1.03</f>
-        <v>60895.66</v>
+        <f t="shared" ref="B57:B61" si="2">B56*1.0159</f>
+        <v>59239.831294000003</v>
       </c>
       <c r="C57" s="11">
         <v>3500</v>
@@ -7854,8 +7854,8 @@
         <f t="shared" ref="AC57:AC61" si="8">AC56*1.03</f>
         <v>526.58832400000006</v>
       </c>
-      <c r="AD57" s="11">
-        <v>2.3E-2</v>
+      <c r="AD57" s="17">
+        <v>1.5900000000000001E-2</v>
       </c>
       <c r="AE57" s="12">
         <v>1</v>
@@ -7891,7 +7891,7 @@
       </c>
       <c r="B58" s="11">
         <f t="shared" si="2"/>
-        <v>62722.529800000004</v>
+        <v>60181.744611574606</v>
       </c>
       <c r="C58" s="11">
         <v>3500</v>
@@ -7977,8 +7977,8 @@
         <f t="shared" si="8"/>
         <v>542.38597372000004</v>
       </c>
-      <c r="AD58" s="11">
-        <v>2.3E-2</v>
+      <c r="AD58" s="17">
+        <v>1.5900000000000001E-2</v>
       </c>
       <c r="AE58" s="12">
         <v>1</v>
@@ -8014,7 +8014,7 @@
       </c>
       <c r="B59" s="11">
         <f t="shared" si="2"/>
-        <v>64604.205694000004</v>
+        <v>61138.634350898647</v>
       </c>
       <c r="C59" s="11">
         <v>3500</v>
@@ -8100,8 +8100,8 @@
         <f t="shared" si="8"/>
         <v>558.65755293160009</v>
       </c>
-      <c r="AD59" s="11">
-        <v>2.3E-2</v>
+      <c r="AD59" s="17">
+        <v>1.5900000000000001E-2</v>
       </c>
       <c r="AE59" s="12">
         <v>1</v>
@@ -8137,7 +8137,7 @@
       </c>
       <c r="B60" s="11">
         <f t="shared" si="2"/>
-        <v>66542.331864820007</v>
+        <v>62110.738637077935</v>
       </c>
       <c r="C60" s="11">
         <v>3500</v>
@@ -8223,8 +8223,8 @@
         <f t="shared" si="8"/>
         <v>575.41727951954806</v>
       </c>
-      <c r="AD60" s="11">
-        <v>2.3E-2</v>
+      <c r="AD60" s="17">
+        <v>1.5900000000000001E-2</v>
       </c>
       <c r="AE60" s="11">
         <v>1.07</v>
@@ -8260,7 +8260,7 @@
       </c>
       <c r="B61" s="11">
         <f t="shared" si="2"/>
-        <v>68538.601820764612</v>
+        <v>63098.299381407473</v>
       </c>
       <c r="C61" s="11">
         <v>3500</v>
@@ -8346,8 +8346,8 @@
         <f t="shared" si="8"/>
         <v>592.67979790513448</v>
       </c>
-      <c r="AD61" s="11">
-        <v>2.3E-2</v>
+      <c r="AD61" s="17">
+        <v>1.5900000000000001E-2</v>
       </c>
       <c r="AE61" s="11">
         <v>1.1399999999999999</v>

</xml_diff>